<commit_message>
✨Adding the fields: receivedAt, planEndDate, filterVersion, deviceProgram to the table of: customerDevice
</commit_message>
<xml_diff>
--- a/lib/deviceToDonator.xlsx
+++ b/lib/deviceToDonator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\yaazoru\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47CB5A5-659B-431A-A241-3D8AA1F1D323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B219729E-7239-4385-82AE-8EDEAC93DC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9F3DF62E-83AB-472E-9D08-CA2C32615E73}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9F3DF62E-83AB-472E-9D08-CA2C32615E73}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -6577,9 +6577,6 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>device_number</t>
   </si>
   <si>
@@ -6644,6 +6641,9 @@
   </si>
   <si>
     <t>שוורצמן</t>
+  </si>
+  <si>
+    <t>receivedAt</t>
   </si>
 </sst>
 </file>
@@ -7286,8 +7286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4CC6D0E-32F5-4CC2-BD07-334C071C9F90}">
   <dimension ref="A1:S391"/>
   <sheetViews>
-    <sheetView rightToLeft="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7310,7 +7310,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2160</v>
@@ -7328,7 +7328,7 @@
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2172</v>
+        <v>2194</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2164</v>
@@ -25640,8 +25640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A20716-F9BD-496B-9CCD-B3DD29AF7F25}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView rightToLeft="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -25666,7 +25666,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2160</v>
@@ -25684,7 +25684,7 @@
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2172</v>
+        <v>2194</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2164</v>
@@ -25734,7 +25734,7 @@
         <v>851221555</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>193</v>
@@ -25749,7 +25749,7 @@
         <v>1387</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>162</v>
@@ -25758,11 +25758,11 @@
         <v>687</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="44" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="O2" s="6">
         <v>930</v>
@@ -25789,10 +25789,10 @@
         <v>254789654</v>
       </c>
       <c r="D3" t="s">
+        <v>2177</v>
+      </c>
+      <c r="E3" t="s">
         <v>2178</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2179</v>
       </c>
       <c r="G3" s="45">
         <v>45608</v>
@@ -25807,13 +25807,13 @@
         <v>112</v>
       </c>
       <c r="K3" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="L3" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="N3" s="46" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="O3">
         <v>800</v>
@@ -25851,16 +25851,16 @@
         <v>421</v>
       </c>
       <c r="K4" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="L4" t="s">
+        <v>2182</v>
+      </c>
+      <c r="M4" t="s">
         <v>2183</v>
       </c>
-      <c r="M4" t="s">
-        <v>2184</v>
-      </c>
       <c r="N4" s="46" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="O4">
         <v>820</v>
@@ -25869,7 +25869,7 @@
         <v>258741203</v>
       </c>
       <c r="Q4" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -25883,13 +25883,13 @@
         <v>258963258</v>
       </c>
       <c r="D5" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="E5" t="s">
         <v>193</v>
       </c>
       <c r="Q5" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -25924,10 +25924,10 @@
         <v>1714</v>
       </c>
       <c r="L6" t="s">
+        <v>2189</v>
+      </c>
+      <c r="N6" s="46" t="s">
         <v>2190</v>
-      </c>
-      <c r="N6" s="46" t="s">
-        <v>2191</v>
       </c>
       <c r="O6">
         <v>880</v>
@@ -25950,10 +25950,10 @@
         <v>258963214</v>
       </c>
       <c r="D7" t="s">
+        <v>2191</v>
+      </c>
+      <c r="E7" t="s">
         <v>2192</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2193</v>
       </c>
       <c r="G7" s="45">
         <v>45628</v>
@@ -25962,7 +25962,7 @@
         <v>677</v>
       </c>
       <c r="I7" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="L7">
         <v>5321478562</v>

</xml_diff>